<commit_message>
update list of herbs
</commit_message>
<xml_diff>
--- a/Category/ingredientInfo.xlsx
+++ b/Category/ingredientInfo.xlsx
@@ -1069,7 +1069,11 @@
           <t>Eryngium foetidum</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
           <t>Earthy</t>
@@ -1081,7 +1085,11 @@
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>

</xml_diff>